<commit_message>
Add Phone Number to Santosh Family
</commit_message>
<xml_diff>
--- a/IPO_NameList_Single_working.xlsx
+++ b/IPO_NameList_Single_working.xlsx
@@ -7538,14 +7538,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -7975,10 +7975,10 @@
   <dimension ref="A1:AD302"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="K91" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="W4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P117" sqref="P117"/>
+      <selection pane="bottomRight" activeCell="AD7" sqref="AD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8015,17 +8015,17 @@
     <col min="30" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:30">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="38"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
@@ -8035,22 +8035,22 @@
       <c r="G1" s="6" t="s">
         <v>390</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="40" t="s">
         <v>391</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="I1" s="40" t="s">
         <v>2337</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="J1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="38" t="s">
+      <c r="K1" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="38"/>
+      <c r="M1" s="40"/>
       <c r="N1" s="43" t="s">
         <v>8</v>
       </c>
@@ -8066,29 +8066,29 @@
       <c r="R1" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="38" t="s">
+      <c r="S1" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="38"/>
-      <c r="U1" s="38"/>
-      <c r="V1" s="38" t="s">
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="W1" s="38"/>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="38"/>
+      <c r="W1" s="40"/>
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
-      <c r="AB1" s="39" t="s">
+      <c r="AB1" s="38" t="s">
         <v>2342</v>
       </c>
-      <c r="AC1" s="40" t="s">
+      <c r="AC1" s="39" t="s">
         <v>2343</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
+    <row r="2" spans="1:30">
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
       <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
@@ -8098,14 +8098,14 @@
       <c r="E2" s="5"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
       <c r="L2" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="38" t="s">
+      <c r="M2" s="40" t="s">
         <v>17</v>
       </c>
       <c r="N2" s="43"/>
@@ -8113,33 +8113,33 @@
       <c r="P2" s="42"/>
       <c r="Q2" s="42"/>
       <c r="R2" s="42"/>
-      <c r="S2" s="38" t="s">
+      <c r="S2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="38" t="s">
+      <c r="T2" s="40" t="s">
         <v>19</v>
       </c>
       <c r="U2" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="38" t="s">
+      <c r="V2" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="W2" s="38"/>
-      <c r="X2" s="38"/>
-      <c r="Y2" s="38"/>
+      <c r="W2" s="40"/>
+      <c r="X2" s="40"/>
+      <c r="Y2" s="40"/>
       <c r="Z2" s="2" t="s">
         <v>700</v>
       </c>
       <c r="AA2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AB2" s="39"/>
-      <c r="AC2" s="40"/>
-    </row>
-    <row r="3" spans="1:29">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="39"/>
+    </row>
+    <row r="3" spans="1:30">
+      <c r="A3" s="40"/>
+      <c r="B3" s="40"/>
       <c r="C3" s="6">
         <v>13010900</v>
       </c>
@@ -8149,19 +8149,19 @@
       <c r="E3" s="3"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
       <c r="N3" s="43"/>
       <c r="O3" s="43"/>
       <c r="P3" s="42"/>
       <c r="Q3" s="42"/>
       <c r="R3" s="42"/>
-      <c r="S3" s="38"/>
-      <c r="T3" s="38"/>
+      <c r="S3" s="40"/>
+      <c r="T3" s="40"/>
       <c r="U3" s="42" t="s">
         <v>20</v>
       </c>
@@ -8183,10 +8183,10 @@
       <c r="AA3" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="AB3" s="39"/>
-      <c r="AC3" s="40"/>
-    </row>
-    <row r="4" spans="1:29">
+      <c r="AB3" s="38"/>
+      <c r="AC3" s="39"/>
+    </row>
+    <row r="4" spans="1:30">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -8258,8 +8258,11 @@
       <c r="AC4" s="1">
         <v>9851111307</v>
       </c>
-    </row>
-    <row r="5" spans="1:29">
+      <c r="AD4" s="1">
+        <v>5520771</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -8333,8 +8336,11 @@
       <c r="AC5" s="1">
         <v>9841281942</v>
       </c>
-    </row>
-    <row r="6" spans="1:29">
+      <c r="AD5" s="1">
+        <v>5520771</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -8406,8 +8412,11 @@
       <c r="AC6" s="1">
         <v>9851111307</v>
       </c>
-    </row>
-    <row r="7" spans="1:29">
+      <c r="AD6" s="1">
+        <v>5520771</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -8481,8 +8490,11 @@
       <c r="AC7" s="1">
         <v>9851111307</v>
       </c>
-    </row>
-    <row r="8" spans="1:29">
+      <c r="AD7" s="1">
+        <v>5520771</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -8551,7 +8563,7 @@
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:30">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -8620,7 +8632,7 @@
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:30">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -8679,7 +8691,7 @@
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:30">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -8748,7 +8760,7 @@
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:30">
       <c r="A12" s="7">
         <v>9</v>
       </c>
@@ -8815,7 +8827,7 @@
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:30">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -8880,7 +8892,7 @@
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:30">
       <c r="A14" s="7">
         <v>11</v>
       </c>
@@ -8945,7 +8957,7 @@
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:30">
       <c r="A15" s="7">
         <v>12</v>
       </c>
@@ -9012,7 +9024,7 @@
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:30">
       <c r="A16" s="7">
         <v>13</v>
       </c>
@@ -27116,6 +27128,13 @@
     <filterColumn colId="23" showButton="0"/>
   </autoFilter>
   <mergeCells count="23">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="J1:J3"/>
+    <mergeCell ref="K1:K3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I1:I3"/>
     <mergeCell ref="AB1:AB3"/>
     <mergeCell ref="AC1:AC3"/>
     <mergeCell ref="V1:Y1"/>
@@ -27132,13 +27151,6 @@
     <mergeCell ref="R1:R3"/>
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="L1:M1"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="J1:J3"/>
-    <mergeCell ref="K1:K3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I1:I3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AB4" r:id="rId1"/>

</xml_diff>

<commit_message>
Add phone number to Maa
</commit_message>
<xml_diff>
--- a/IPO_NameList_Single_working.xlsx
+++ b/IPO_NameList_Single_working.xlsx
@@ -7538,14 +7538,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -7975,10 +7975,10 @@
   <dimension ref="A1:AD302"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="W4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="U4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AD7" sqref="AD7"/>
+      <selection pane="bottomRight" activeCell="AD19" sqref="AD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8016,16 +8016,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40"/>
+      <c r="D1" s="38"/>
       <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
@@ -8035,22 +8035,22 @@
       <c r="G1" s="6" t="s">
         <v>390</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="38" t="s">
         <v>391</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="38" t="s">
         <v>2337</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="J1" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="40" t="s">
+      <c r="K1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="40" t="s">
+      <c r="L1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="40"/>
+      <c r="M1" s="38"/>
       <c r="N1" s="43" t="s">
         <v>8</v>
       </c>
@@ -8066,29 +8066,29 @@
       <c r="R1" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="40" t="s">
+      <c r="S1" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="40"/>
-      <c r="U1" s="40"/>
-      <c r="V1" s="40" t="s">
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="W1" s="40"/>
-      <c r="X1" s="40"/>
-      <c r="Y1" s="40"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
-      <c r="AB1" s="38" t="s">
+      <c r="AB1" s="39" t="s">
         <v>2342</v>
       </c>
-      <c r="AC1" s="39" t="s">
+      <c r="AC1" s="40" t="s">
         <v>2343</v>
       </c>
     </row>
     <row r="2" spans="1:30">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
       <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
@@ -8098,14 +8098,14 @@
       <c r="E2" s="5"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
       <c r="L2" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="40" t="s">
+      <c r="M2" s="38" t="s">
         <v>17</v>
       </c>
       <c r="N2" s="43"/>
@@ -8113,33 +8113,33 @@
       <c r="P2" s="42"/>
       <c r="Q2" s="42"/>
       <c r="R2" s="42"/>
-      <c r="S2" s="40" t="s">
+      <c r="S2" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="40" t="s">
+      <c r="T2" s="38" t="s">
         <v>19</v>
       </c>
       <c r="U2" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="40" t="s">
+      <c r="V2" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="W2" s="40"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="40"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="38"/>
       <c r="Z2" s="2" t="s">
         <v>700</v>
       </c>
       <c r="AA2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AB2" s="38"/>
-      <c r="AC2" s="39"/>
+      <c r="AB2" s="39"/>
+      <c r="AC2" s="40"/>
     </row>
     <row r="3" spans="1:30">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
       <c r="C3" s="6">
         <v>13010900</v>
       </c>
@@ -8149,19 +8149,19 @@
       <c r="E3" s="3"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
       <c r="N3" s="43"/>
       <c r="O3" s="43"/>
       <c r="P3" s="42"/>
       <c r="Q3" s="42"/>
       <c r="R3" s="42"/>
-      <c r="S3" s="40"/>
-      <c r="T3" s="40"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
       <c r="U3" s="42" t="s">
         <v>20</v>
       </c>
@@ -8183,8 +8183,8 @@
       <c r="AA3" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="AB3" s="38"/>
-      <c r="AC3" s="39"/>
+      <c r="AB3" s="39"/>
+      <c r="AC3" s="40"/>
     </row>
     <row r="4" spans="1:30">
       <c r="A4" s="7">
@@ -8759,6 +8759,9 @@
       <c r="Y11" s="6"/>
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
+      <c r="AD11" s="1">
+        <v>5520771</v>
+      </c>
     </row>
     <row r="12" spans="1:30">
       <c r="A12" s="7">
@@ -27128,13 +27131,6 @@
     <filterColumn colId="23" showButton="0"/>
   </autoFilter>
   <mergeCells count="23">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="J1:J3"/>
-    <mergeCell ref="K1:K3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I1:I3"/>
     <mergeCell ref="AB1:AB3"/>
     <mergeCell ref="AC1:AC3"/>
     <mergeCell ref="V1:Y1"/>
@@ -27151,6 +27147,13 @@
     <mergeCell ref="R1:R3"/>
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="L1:M1"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="J1:J3"/>
+    <mergeCell ref="K1:K3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I1:I3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AB4" r:id="rId1"/>

</xml_diff>